<commit_message>
Added tests for JSON Model Structure
</commit_message>
<xml_diff>
--- a/testChecklist.xlsx
+++ b/testChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw6_reqres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC45BE5-034A-4B3D-A6A5-EB2644177244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBD815-3374-45A2-8DE8-1E31416E66CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0D155417-BCE7-4DAB-8DC1-E59CBFA23152}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Reqres Testing Matrix</t>
   </si>
@@ -155,10 +155,40 @@
     <t>Body: Only Email</t>
   </si>
   <si>
-    <t>Schema</t>
-  </si>
-  <si>
-    <t>Full Response</t>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>ListUsers</t>
+  </si>
+  <si>
+    <t>SingleUser</t>
+  </si>
+  <si>
+    <t>SingleResource</t>
+  </si>
+  <si>
+    <t>ListResources</t>
+  </si>
+  <si>
+    <t>RegUser</t>
+  </si>
+  <si>
+    <t>JobUserCreated</t>
+  </si>
+  <si>
+    <t>JobUserUpdated</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>Check Exact</t>
+  </si>
+  <si>
+    <t>Check Error</t>
   </si>
 </sst>
 </file>
@@ -517,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3950A36E-BDE3-4628-BDBF-51E5AEE8F3B6}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,12 +558,12 @@
     <col min="2" max="2" width="29.6328125" customWidth="1"/>
     <col min="3" max="3" width="25.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="7" width="13.453125" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -564,10 +594,13 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -580,8 +613,11 @@
       <c r="D4" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -594,8 +630,14 @@
       <c r="D5" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -608,8 +650,11 @@
       <c r="D6" s="1">
         <v>404</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -622,8 +667,11 @@
       <c r="D7" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -636,8 +684,14 @@
       <c r="D8" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -650,8 +704,11 @@
       <c r="D9" s="1">
         <v>404</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -664,11 +721,14 @@
       <c r="D10" s="1">
         <v>201</v>
       </c>
-      <c r="G10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -681,11 +741,14 @@
       <c r="D11" s="1">
         <v>200</v>
       </c>
-      <c r="G11" t="s">
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -698,11 +761,14 @@
       <c r="D12" s="1">
         <v>200</v>
       </c>
-      <c r="G12" t="s">
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -716,7 +782,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -729,11 +795,14 @@
       <c r="D14" s="1">
         <v>200</v>
       </c>
-      <c r="G14" t="s">
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -747,10 +816,13 @@
         <v>400</v>
       </c>
       <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -763,11 +835,14 @@
       <c r="D16" s="1">
         <v>200</v>
       </c>
-      <c r="G16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -781,10 +856,13 @@
         <v>400</v>
       </c>
       <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -796,6 +874,9 @@
       </c>
       <c r="D18" s="1">
         <v>200</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed tests for Error Messages
</commit_message>
<xml_diff>
--- a/testChecklist.xlsx
+++ b/testChecklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Java\hw6_reqres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBBD815-3374-45A2-8DE8-1E31416E66CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19A6ACD-D454-4450-910C-588C3A624DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0D155417-BCE7-4DAB-8DC1-E59CBFA23152}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>Reqres Testing Matrix</t>
   </si>
@@ -182,13 +182,19 @@
     <t>JobUserUpdated</t>
   </si>
   <si>
-    <t>Error message</t>
-  </si>
-  <si>
-    <t>Check Exact</t>
-  </si>
-  <si>
-    <t>Check Error</t>
+    <t>Error messages</t>
+  </si>
+  <si>
+    <t>Error: User without email</t>
+  </si>
+  <si>
+    <t>Errors: User without email, user without password</t>
+  </si>
+  <si>
+    <t>Check Full JSON</t>
+  </si>
+  <si>
+    <t>Check Page 2: some values, full JSON</t>
   </si>
 </sst>
 </file>
@@ -230,9 +236,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3950A36E-BDE3-4628-BDBF-51E5AEE8F3B6}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,7 +577,8 @@
     <col min="3" max="3" width="25.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.54296875" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" customWidth="1"/>
-    <col min="6" max="7" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
     <col min="8" max="8" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,21 +619,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>200</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -633,8 +655,8 @@
       <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
-        <v>49</v>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -650,9 +672,6 @@
       <c r="D6" s="1">
         <v>404</v>
       </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -687,8 +706,8 @@
       <c r="E8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F8" t="s">
-        <v>49</v>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -704,9 +723,6 @@
       <c r="D9" s="1">
         <v>404</v>
       </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -802,20 +818,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>400</v>
       </c>
-      <c r="G15" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H15" t="s">
@@ -855,8 +873,8 @@
       <c r="D17" s="1">
         <v>400</v>
       </c>
-      <c r="G17" t="s">
-        <v>50</v>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="H17" t="s">
         <v>38</v>

</xml_diff>